<commit_message>
Update version numbers for forms
</commit_message>
<xml_diff>
--- a/app/config/tables/colombia_delivery/forms/colombia_delivery/colombia_delivery.xlsx
+++ b/app/config/tables/colombia_delivery/forms/colombia_delivery/colombia_delivery.xlsx
@@ -1840,7 +1840,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
@@ -1886,7 +1886,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="17">
-        <v>20190604</v>
+        <v>20190609</v>
       </c>
       <c r="C3"/>
     </row>

</xml_diff>

<commit_message>
Pre-populate custom forms with dept and pam fields only if the custom forms have the fields
</commit_message>
<xml_diff>
--- a/app/config/tables/colombia_delivery/forms/colombia_delivery/colombia_delivery.xlsx
+++ b/app/config/tables/colombia_delivery/forms/colombia_delivery/colombia_delivery.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19150" windowHeight="5570" tabRatio="989" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19150" windowHeight="5570" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="271">
   <si>
     <t>clause</t>
   </si>
@@ -220,9 +220,6 @@
     <t>activity_date</t>
   </si>
   <si>
-    <t>Departamento:</t>
-  </si>
-  <si>
     <t>Selecciona el fianciador de la actividad:</t>
   </si>
   <si>
@@ -232,15 +229,6 @@
     <t>display.hint.text.es</t>
   </si>
   <si>
-    <t>Department:</t>
-  </si>
-  <si>
-    <t>Punto de Atención a Migrantes:</t>
-  </si>
-  <si>
-    <t>Point of Attention to Migrants:</t>
-  </si>
-  <si>
     <t>pam</t>
   </si>
   <si>
@@ -256,22 +244,10 @@
     <t>display.constraint_message.text.es</t>
   </si>
   <si>
-    <t>Por favor, introduzca el Departamento</t>
-  </si>
-  <si>
     <t>Por favor, introduzca el Proyecto en el que se enmarca la actividad</t>
   </si>
   <si>
-    <t>Please enter the department</t>
-  </si>
-  <si>
     <t>Please enter the Project in which the activity is framed</t>
-  </si>
-  <si>
-    <t>Por favor, introduzca el Punto de Atención a Migrantes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter the Point of Attention to Migrants: </t>
   </si>
   <si>
     <t>Cucuta_IPS</t>
@@ -864,9 +840,6 @@
   <si>
     <t xml:space="preserve">
 Inglés</t>
-  </si>
-  <si>
-    <t>choice_item.filter_value === data('department')</t>
   </si>
   <si>
     <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
@@ -1111,7 +1084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1153,8 +1126,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1165,7 +1136,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1555,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
@@ -1569,7 +1539,7 @@
     <col min="4" max="4" width="32.08203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="37.5" style="4" customWidth="1"/>
     <col min="6" max="8" width="35.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="50.1640625" style="38" customWidth="1"/>
+    <col min="9" max="9" width="50.1640625" style="36" customWidth="1"/>
     <col min="10" max="10" width="25.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="20.1640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="17.1640625" style="1" customWidth="1"/>
@@ -1579,7 +1549,7 @@
     <col min="16" max="16" width="27.58203125" customWidth="1"/>
     <col min="17" max="17" width="47.4140625" customWidth="1"/>
     <col min="18" max="18" width="30.6640625" customWidth="1"/>
-    <col min="19" max="19" width="18.1640625" style="45" customWidth="1"/>
+    <col min="19" max="19" width="18.1640625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -1601,13 +1571,13 @@
       <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="35" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="10" t="s">
@@ -1619,26 +1589,26 @@
       <c r="L1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="43" t="s">
+      <c r="N1" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="R1" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="S1" s="44" t="s">
-        <v>123</v>
+      <c r="Q1" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="41" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -1660,174 +1630,89 @@
         <v>11</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
-      <c r="I3" s="52" t="s">
-        <v>257</v>
-      </c>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
+      <c r="I3" s="49" t="s">
+        <v>249</v>
+      </c>
+      <c r="M3" s="1" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="31" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" s="51" t="s">
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>255</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="J4" s="56"/>
+      <c r="L4" s="57"/>
       <c r="M4" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" s="33" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="54" t="s">
-        <v>11</v>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="58" t="s">
-        <v>276</v>
-      </c>
-      <c r="J5" s="59"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>274</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="J6" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="M6" s="1" t="b">
+        <v>264</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="J5" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="M5" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
+      <c r="N5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="39"/>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="39"/>
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="11"/>
-      <c r="J9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M9" s="1" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="S9" s="45" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="39"/>
-      <c r="M10"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="37"/>
+      <c r="M6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1839,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1863,13 +1748,13 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="F1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1877,7 +1762,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C2"/>
     </row>
@@ -1895,7 +1780,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C4"/>
     </row>
@@ -1905,32 +1790,32 @@
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D5" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="16" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E6" t="s">
-        <v>262</v>
-      </c>
-      <c r="F6" s="53" t="s">
-        <v>264</v>
+        <v>254</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="16" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="E7" t="s">
-        <v>263</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>265</v>
+        <v>255</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -1943,15 +1828,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="51.1640625" style="3" customWidth="1"/>
-    <col min="3" max="9" width="8.6640625" style="1"/>
+    <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
+    <col min="4" max="9" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1964,7 +1850,9 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="21" t="s">
+        <v>10</v>
+      </c>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -1976,10 +1864,12 @@
         <v>15</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C2"/>
-      <c r="D2" s="21"/>
+      <c r="D2" s="21" t="b">
+        <v>1</v>
+      </c>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
@@ -1994,7 +1884,9 @@
         <v>57</v>
       </c>
       <c r="C3"/>
-      <c r="D3" s="21"/>
+      <c r="D3" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -2009,7 +1901,9 @@
         <v>59</v>
       </c>
       <c r="C4"/>
-      <c r="D4" s="21"/>
+      <c r="D4" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
@@ -2021,10 +1915,12 @@
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C5"/>
-      <c r="D5" s="21"/>
+      <c r="D5" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -2036,7 +1932,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="D6" s="22" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2072,1588 +1971,1588 @@
         <v>20</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>125</v>
+        <v>247</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B3" s="46" t="s">
-        <v>126</v>
+        <v>247</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>255</v>
-      </c>
-      <c r="B4" s="46" t="s">
-        <v>127</v>
+        <v>247</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B5" s="46" t="s">
-        <v>129</v>
+        <v>247</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>255</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>131</v>
+        <v>247</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>133</v>
+        <v>247</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>255</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>134</v>
+        <v>247</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>255</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>135</v>
+        <v>247</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>127</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>255</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>137</v>
+        <v>247</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>255</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>138</v>
+        <v>247</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>130</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>255</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>140</v>
+        <v>247</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>132</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>255</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>142</v>
+        <v>247</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>134</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>255</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>143</v>
+        <v>247</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>255</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>80</v>
+        <v>247</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>255</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>101</v>
+        <v>247</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>255</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>108</v>
+        <v>247</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>100</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>255</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>111</v>
+        <v>247</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>255</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" s="47"/>
+        <v>247</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="44"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>255</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>121</v>
+        <v>247</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="36"/>
+      <c r="B21" s="34"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>275</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>147</v>
+        <v>266</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>139</v>
       </c>
       <c r="C22" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>275</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>148</v>
+        <v>266</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>275</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="E24" s="47"/>
+        <v>266</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>275</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>151</v>
+        <v>266</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>143</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>275</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>153</v>
+        <v>266</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>275</v>
-      </c>
-      <c r="B27" s="36" t="s">
-        <v>155</v>
+        <v>266</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>275</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="C28" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="D28" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="E28" s="47"/>
+        <v>266</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="44"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>275</v>
-      </c>
-      <c r="B29" s="36" t="s">
-        <v>158</v>
+        <v>266</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>150</v>
       </c>
       <c r="C29" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>275</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>160</v>
+        <v>266</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>152</v>
       </c>
       <c r="C30" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D30" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>275</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>162</v>
+        <v>266</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>154</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>275</v>
-      </c>
-      <c r="B32" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="D32" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="E32" s="47"/>
+        <v>266</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="44"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>275</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>166</v>
+        <v>266</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>158</v>
       </c>
       <c r="C33" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>275</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>167</v>
+        <v>266</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>159</v>
       </c>
       <c r="C34" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D34" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>275</v>
-      </c>
-      <c r="B35" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="D35" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="E35" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="45"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>275</v>
-      </c>
-      <c r="B36" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="C36" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="E36" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B36" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="45"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>275</v>
-      </c>
-      <c r="B37" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="C37" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="D37" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="E37" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B37" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" s="45"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>275</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="C38" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="E38" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B38" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" s="45"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>275</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="C39" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="D39" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="E39" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B39" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="45"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>275</v>
-      </c>
-      <c r="B40" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="C40" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="E40" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B40" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="45"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>275</v>
-      </c>
-      <c r="B41" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="C41" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="D41" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="E41" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B41" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="E41" s="45"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>275</v>
-      </c>
-      <c r="B42" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="C42" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="D42" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="E42" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B42" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="E42" s="45"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>275</v>
-      </c>
-      <c r="B43" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="C43" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="D43" s="48" t="s">
-        <v>182</v>
-      </c>
-      <c r="E43" s="48"/>
+        <v>266</v>
+      </c>
+      <c r="B43" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E43" s="45"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>275</v>
-      </c>
-      <c r="B44" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="C44" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="D44" s="49" t="s">
-        <v>183</v>
-      </c>
-      <c r="E44" s="49"/>
+        <v>266</v>
+      </c>
+      <c r="B44" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="D44" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" s="46"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>275</v>
-      </c>
-      <c r="B45" s="49" t="s">
-        <v>184</v>
-      </c>
-      <c r="C45" s="49" t="s">
-        <v>184</v>
-      </c>
-      <c r="D45" s="49" t="s">
-        <v>184</v>
-      </c>
-      <c r="E45" s="49"/>
+        <v>266</v>
+      </c>
+      <c r="B45" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="E45" s="46"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>275</v>
-      </c>
-      <c r="B46" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="C46" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="D46" s="49" t="s">
-        <v>185</v>
-      </c>
-      <c r="E46" s="49"/>
+        <v>266</v>
+      </c>
+      <c r="B46" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="D46" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="E46" s="46"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>275</v>
-      </c>
-      <c r="B47" s="49" t="s">
-        <v>186</v>
-      </c>
-      <c r="C47" s="49" t="s">
-        <v>186</v>
-      </c>
-      <c r="D47" s="49" t="s">
-        <v>186</v>
-      </c>
-      <c r="E47" s="49"/>
+        <v>266</v>
+      </c>
+      <c r="B47" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="D47" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" s="46"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>275</v>
-      </c>
-      <c r="B48" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="D48" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E48" s="43"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="D50" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="E50" s="43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="D51" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="E52" s="43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="D53" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="D48" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="E48" s="46"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B49" s="46"/>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="46" t="s">
+      <c r="E53" s="43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="C50" s="46" t="s">
+      <c r="C54" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="D50" s="46" t="s">
+      <c r="D54" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="E50" s="46" t="s">
+      <c r="E54" s="43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="D55" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="E55" s="43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="C56" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="D56" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="E56" s="43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D57" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="E57" s="46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="E58" s="46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="C59" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="D59" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="E59" s="46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="E60" s="46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="D61" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="E61" s="46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="C62" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="E62" s="46" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" s="46" t="s">
-        <v>190</v>
-      </c>
-      <c r="C51" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="D51" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="E51" s="46" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="46" t="s">
-        <v>192</v>
-      </c>
-      <c r="C52" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="D52" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="E52" s="46" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="C53" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D53" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="E53" s="46" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="C63" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="E63" s="46" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="C54" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="D54" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="E54" s="46" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="D64" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="E64" s="46" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="46" t="s">
-        <v>198</v>
-      </c>
-      <c r="C55" s="46" t="s">
-        <v>199</v>
-      </c>
-      <c r="D55" s="46" t="s">
-        <v>199</v>
-      </c>
-      <c r="E55" s="46" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="C56" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D56" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="E56" s="46" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="49" t="s">
-        <v>202</v>
-      </c>
-      <c r="C57" s="49" t="s">
-        <v>203</v>
-      </c>
-      <c r="D57" s="49" t="s">
-        <v>203</v>
-      </c>
-      <c r="E57" s="49" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="49" t="s">
-        <v>204</v>
-      </c>
-      <c r="C58" s="49" t="s">
-        <v>205</v>
-      </c>
-      <c r="D58" s="49" t="s">
-        <v>205</v>
-      </c>
-      <c r="E58" s="49" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" s="49" t="s">
-        <v>206</v>
-      </c>
-      <c r="C59" s="49" t="s">
-        <v>207</v>
-      </c>
-      <c r="D59" s="49" t="s">
-        <v>207</v>
-      </c>
-      <c r="E59" s="49" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="C65" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="D65" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="E65" s="46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="C66" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="D66" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="E66" s="46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="C67" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="D67" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="E67" s="46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="C68" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="D68" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="E68" s="46" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" s="49" t="s">
-        <v>208</v>
-      </c>
-      <c r="C60" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="D60" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="E60" s="49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="49" t="s">
-        <v>210</v>
-      </c>
-      <c r="C61" s="49" t="s">
-        <v>211</v>
-      </c>
-      <c r="D61" s="49" t="s">
-        <v>211</v>
-      </c>
-      <c r="E61" s="49" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B62" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="C62" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="D62" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="E62" s="49" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B63" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="C63" s="49" t="s">
-        <v>215</v>
-      </c>
-      <c r="D63" s="49" t="s">
-        <v>215</v>
-      </c>
-      <c r="E63" s="49" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="C69" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="D69" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="E69" s="46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="C70" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="D70" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="E70" s="46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B71" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="C71" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="D71" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="E71" s="46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B72" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="C72" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="D72" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="E72" s="46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B73" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="C73" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="D73" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="E73" s="46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="D74" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="E74" s="46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B75" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="C75" s="46" t="s">
+        <v>231</v>
+      </c>
+      <c r="D75" s="46" t="s">
+        <v>231</v>
+      </c>
+      <c r="E75" s="46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B76" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="C76" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="D76" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="E76" s="43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B77" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="D77" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="E77" s="46" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B64" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="C64" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="D64" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="E64" s="49" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B65" s="46" t="s">
-        <v>218</v>
-      </c>
-      <c r="C65" s="49" t="s">
-        <v>219</v>
-      </c>
-      <c r="D65" s="49" t="s">
-        <v>219</v>
-      </c>
-      <c r="E65" s="49" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B66" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="C66" s="49" t="s">
-        <v>221</v>
-      </c>
-      <c r="D66" s="49" t="s">
-        <v>221</v>
-      </c>
-      <c r="E66" s="49" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B67" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="C67" s="49" t="s">
-        <v>223</v>
-      </c>
-      <c r="D67" s="49" t="s">
-        <v>223</v>
-      </c>
-      <c r="E67" s="49" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B68" s="49" t="s">
-        <v>224</v>
-      </c>
-      <c r="C68" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="D68" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="E68" s="49" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B69" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="C69" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="D69" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="E69" s="49" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="C70" s="49" t="s">
-        <v>229</v>
-      </c>
-      <c r="D70" s="49" t="s">
-        <v>229</v>
-      </c>
-      <c r="E70" s="49" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B71" s="49" t="s">
-        <v>230</v>
-      </c>
-      <c r="C71" s="49" t="s">
-        <v>231</v>
-      </c>
-      <c r="D71" s="49" t="s">
-        <v>231</v>
-      </c>
-      <c r="E71" s="49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B72" s="49" t="s">
-        <v>232</v>
-      </c>
-      <c r="C72" s="49" t="s">
-        <v>233</v>
-      </c>
-      <c r="D72" s="49" t="s">
-        <v>233</v>
-      </c>
-      <c r="E72" s="49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B73" s="49" t="s">
-        <v>234</v>
-      </c>
-      <c r="C73" s="49" t="s">
-        <v>235</v>
-      </c>
-      <c r="D73" s="49" t="s">
-        <v>235</v>
-      </c>
-      <c r="E73" s="49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B74" s="46" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B78" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="C74" s="49" t="s">
+      <c r="C78" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="D74" s="49" t="s">
+      <c r="D78" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="E74" s="49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B75" s="46" t="s">
+      <c r="E78" s="46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B79" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="C75" s="49" t="s">
+      <c r="C79" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="D75" s="49" t="s">
+      <c r="D79" s="46" t="s">
         <v>239</v>
       </c>
-      <c r="E75" s="49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B76" s="46" t="s">
+      <c r="E79" s="46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="46" t="s">
         <v>240</v>
       </c>
-      <c r="C76" s="46" t="s">
+      <c r="C80" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="D76" s="46" t="s">
+      <c r="D80" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="E76" s="46" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B77" s="46" t="s">
+      <c r="E80" s="46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B81" s="46" t="s">
         <v>242</v>
       </c>
-      <c r="C77" s="49" t="s">
+      <c r="C81" s="46" t="s">
         <v>243</v>
       </c>
-      <c r="D77" s="49" t="s">
+      <c r="D81" s="46" t="s">
         <v>243</v>
       </c>
-      <c r="E77" s="49" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B78" s="46" t="s">
+      <c r="E81" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B82" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="C78" s="49" t="s">
+      <c r="C82" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="D78" s="49" t="s">
+      <c r="D82" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="E78" s="49" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B79" s="49" t="s">
-        <v>246</v>
-      </c>
-      <c r="C79" s="49" t="s">
-        <v>247</v>
-      </c>
-      <c r="D79" s="49" t="s">
-        <v>247</v>
-      </c>
-      <c r="E79" s="49" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B80" s="49" t="s">
-        <v>248</v>
-      </c>
-      <c r="C80" s="49" t="s">
-        <v>249</v>
-      </c>
-      <c r="D80" s="49" t="s">
-        <v>249</v>
-      </c>
-      <c r="E80" s="49" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B81" s="49" t="s">
-        <v>250</v>
-      </c>
-      <c r="C81" s="49" t="s">
-        <v>251</v>
-      </c>
-      <c r="D81" s="49" t="s">
-        <v>251</v>
-      </c>
-      <c r="E81" s="49" t="s">
+      <c r="E82" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B83" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C83" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D83" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E83" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C84" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D84" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E84" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C85" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D85" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E85" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B86" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C86" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D86" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="E86" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B87" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C87" s="46" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B82" s="49" t="s">
-        <v>252</v>
-      </c>
-      <c r="C82" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="D82" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="E82" s="49" t="s">
+      <c r="D87" s="46" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B83" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C83" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="D83" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="E83" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B84" s="49" t="s">
+      <c r="E87" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B88" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="49" t="s">
+      <c r="C88" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D84" s="49" t="s">
+      <c r="D88" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="E84" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B85" s="49" t="s">
+      <c r="E88" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="49" t="s">
+      <c r="C89" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="D85" s="49" t="s">
+      <c r="D89" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="E85" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B86" s="49" t="s">
+      <c r="E89" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B90" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="C86" s="49" t="s">
+      <c r="C90" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="D86" s="49" t="s">
+      <c r="D90" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E86" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B87" s="49" t="s">
+      <c r="E90" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B91" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="C87" s="49" t="s">
+      <c r="C91" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="D87" s="49" t="s">
+      <c r="D91" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="E87" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B88" s="49" t="s">
+      <c r="E91" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B92" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C88" s="49" t="s">
+      <c r="C92" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D88" s="49" t="s">
+      <c r="D92" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B89" s="49" t="s">
+      <c r="E92" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B93" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C89" s="49" t="s">
+      <c r="C93" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="49" t="s">
+      <c r="D93" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="E89" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B90" s="49" t="s">
+      <c r="E93" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="C90" s="49" t="s">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B94" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="D90" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="E90" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B91" s="49" t="s">
+      <c r="C94" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="C91" s="49" t="s">
+      <c r="D94" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E94" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B95" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="D91" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="E91" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B92" s="49" t="s">
+      <c r="C95" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C92" s="49" t="s">
+      <c r="D95" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="E95" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B96" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="D92" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="E92" s="49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B93" s="49" t="s">
+      <c r="C96" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="C93" s="49" t="s">
+      <c r="D96" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="E96" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="D93" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="E93" s="49" t="s">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B97" s="46" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B94" s="49" t="s">
+      <c r="C97" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="C94" s="49" t="s">
+      <c r="D97" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="E97" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="D94" s="49" t="s">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B98" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C98" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="E98" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="E94" s="49" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B95" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="C95" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="D95" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="E95" s="49" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B96" s="49" t="s">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B99" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="C96" s="49" t="s">
+      <c r="C99" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="D96" s="49" t="s">
+      <c r="D99" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="E96" s="49" t="s">
+      <c r="E99" s="46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100" s="46" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B97" s="49" t="s">
+      <c r="C100" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="C97" s="51" t="s">
+      <c r="D100" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="E100" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="D97" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="E97" s="51" t="s">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B101" s="46" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B98" s="49" t="s">
+      <c r="C101" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="C98" s="49" t="s">
+      <c r="D101" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="E101" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="D98" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="E98" s="49" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B99" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="C99" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="D99" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="E99" s="49" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B100" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="C100" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="D100" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="E100" s="49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B101" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="C101" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="D101" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="E101" s="49" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" s="46"/>
-      <c r="B102" s="49"/>
-      <c r="C102" s="49"/>
-      <c r="D102" s="49"/>
-      <c r="E102" s="49"/>
+      <c r="A102" s="43"/>
+      <c r="B102" s="46"/>
+      <c r="C102" s="46"/>
+      <c r="D102" s="46"/>
+      <c r="E102" s="46"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>254</v>
-      </c>
-      <c r="B103" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="C103" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="D103" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="E103" s="49"/>
+        <v>246</v>
+      </c>
+      <c r="B103" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C103" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="E103" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3687,8 +3586,8 @@
       <c r="A2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>256</v>
+      <c r="B2" s="31" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3924,27 +3823,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>